<commit_message>
Indigenous school attendance text fixes May31#16-18
</commit_message>
<xml_diff>
--- a/dashboard_loader/indigenous_mortality_uploader/indigenous_mortality.xlsx
+++ b/dashboard_loader/indigenous_mortality_uploader/indigenous_mortality.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" state="visible" r:id="rId2"/>
@@ -155,7 +155,7 @@
     <t xml:space="preserve">Notes</t>
   </si>
   <si>
-    <t xml:space="preserve">Indigenous mortality rates are presented for the five jurisdictions with sufficient quality Indigenous identification in mortality data to publish (NSW, Qld, WA, SA and NT). Four jurisdictions have agreed mortality trajectories to support this target (NSW, Qld, SA and NT) and these are not on track. </t>
+    <t xml:space="preserve">Indigenous mortality rates are presented for the five jurisdictions with evidence of sufficient levels of Indigenous identification and number of deaths to publish (NSW, Qld, WA, SA and NT). Four jurisdictions have agreed mortality trajectories to support this target (NSW, Qld, SA and NT) and these are not on track. </t>
   </si>
   <si>
     <t xml:space="preserve">For 2015 data, the Queensland Registry of Births, Deaths and Marriages included Medical Certificate of Cause of Death information for the first time to contribute to the Indigenous status data item. This data improvement was associated with a decrease in the number of deaths for which the Indigenous status was 'not stated' and an increase in the number of deaths identified as Indigenous in Queensland. This change in method means that time series data for Queensland are not directly comparable and caution should be used in interpreting the trend.</t>
@@ -468,7 +468,7 @@
   </sheetPr>
   <dimension ref="A1:T149"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="C1" activeCellId="0" sqref="C1"/>
@@ -4162,8 +4162,8 @@
   </sheetPr>
   <dimension ref="A1:B12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4224,7 +4224,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="39.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>

</xml_diff>